<commit_message>
Added 2019 Player Attributes files; Finished 2019 pay adjustment calculations; After much testing, almost have all positional generators hitting target rating distribution ranges. Hence, many changes to positional generator utility files.
</commit_message>
<xml_diff>
--- a/docs/Pay Calculations/2018/Contracts Comparison 2018_01_09.xlsx
+++ b/docs/Pay Calculations/2018/Contracts Comparison 2018_01_09.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Gaming\madden_08_updater\docs\2017_12 Debugging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gaming\madden_08_updater\docs\Pay Calculations\2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10395"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -463,19 +463,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" customWidth="1"/>
+    <col min="3" max="4" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -489,7 +489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -504,7 +504,7 @@
         <v>43.01075268817204</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -519,11 +519,11 @@
         <v>59.187006131074696</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -538,7 +538,7 @@
         <v>24.390243902439025</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -553,11 +553,11 @@
         <v>76.294032961929616</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -572,7 +572,7 @@
         <v>49.462365591397848</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -587,11 +587,11 @@
         <v>73.481481481481481</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -620,27 +620,27 @@
         <v>38.876033057851238</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -659,7 +659,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -667,32 +667,32 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -703,7 +703,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>30</v>
       </c>
@@ -711,7 +711,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>32</v>
       </c>
@@ -719,7 +719,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -727,7 +727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>35</v>
       </c>

</xml_diff>